<commit_message>
Actualizo cambios de los nombres
</commit_message>
<xml_diff>
--- a/Proyecto/tablaIndexada.xlsx
+++ b/Proyecto/tablaIndexada.xlsx
@@ -27,10 +27,10 @@
     <t>Tornillo</t>
   </si>
   <si>
+    <t>Alcayata</t>
+  </si>
+  <si>
     <t>Armella</t>
-  </si>
-  <si>
-    <t>Arandela</t>
   </si>
   <si>
     <t>Cola de pato</t>

</xml_diff>

<commit_message>
Creacion de las bases adecuadas
Ya genera la indexada y no indexada
</commit_message>
<xml_diff>
--- a/Proyecto/tablaIndexada.xlsx
+++ b/Proyecto/tablaIndexada.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Data_carac_1</t>
   </si>
@@ -34,6 +34,36 @@
   </si>
   <si>
     <t>Cola de pato</t>
+  </si>
+  <si>
+    <t>Rondana y tornillo</t>
+  </si>
+  <si>
+    <t>Rondana y alcayata</t>
+  </si>
+  <si>
+    <t>Rondana y cola de pato</t>
+  </si>
+  <si>
+    <t>Rondana y Armella</t>
+  </si>
+  <si>
+    <t>Tornillo y alcayata</t>
+  </si>
+  <si>
+    <t>Tornillo y armella</t>
+  </si>
+  <si>
+    <t>Tornillo y cola de pato</t>
+  </si>
+  <si>
+    <t>Alcayata y armella</t>
+  </si>
+  <si>
+    <t>Alcayata y cola de pato</t>
+  </si>
+  <si>
+    <t>Armella y cola de pato</t>
   </si>
   <si>
     <t>Data_carac_2</t>
@@ -97,10 +127,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D17"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="true"/>
+    <col min="1" max="1" width="21.42578125" customWidth="true"/>
     <col min="2" max="2" width="12.5703125" customWidth="true"/>
     <col min="3" max="3" width="12.7109375" customWidth="true"/>
     <col min="4" max="4" width="13" customWidth="true"/>
@@ -111,13 +141,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">
@@ -125,13 +155,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
@@ -153,13 +183,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="0">
-        <v>487.53333333333336</v>
+        <v>715.39999999999998</v>
       </c>
       <c r="C4" s="0">
-        <v>0.27333522522908826</v>
+        <v>0.30672820213309454</v>
       </c>
       <c r="D4" s="0">
-        <v>692.20000000000005</v>
+        <v>1006.8666666666667</v>
       </c>
     </row>
     <row r="5">
@@ -167,13 +197,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="0">
-        <v>697.86666666666667</v>
+        <v>812.20000000000005</v>
       </c>
       <c r="C5" s="0">
-        <v>0.28293152163201019</v>
+        <v>0.34647876166006103</v>
       </c>
       <c r="D5" s="0">
-        <v>1081.6666666666667</v>
+        <v>1217.8</v>
       </c>
     </row>
     <row r="6">
@@ -181,13 +211,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="0">
-        <v>910.5333333333333</v>
+        <v>829.86666666666667</v>
       </c>
       <c r="C6" s="0">
-        <v>0.23938398976237873</v>
+        <v>0.18865995273339869</v>
       </c>
       <c r="D6" s="0">
-        <v>1864.0666666666666</v>
+        <v>1995.5999999999999</v>
       </c>
     </row>
     <row r="7">
@@ -195,13 +225,153 @@
         <v>6</v>
       </c>
       <c r="B7" s="0">
-        <v>1443.5999999999999</v>
+        <v>1862</v>
       </c>
       <c r="C7" s="0">
-        <v>0.41130781546728473</v>
+        <v>0.54403717165424115</v>
       </c>
       <c r="D7" s="0">
-        <v>2277.1999999999998</v>
+        <v>2427.1999999999998</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0">
+        <v>1733</v>
+      </c>
+      <c r="C8" s="0">
+        <v>0.63340083202085984</v>
+      </c>
+      <c r="D8" s="0">
+        <v>1979.0666666666666</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0">
+        <v>1371.5333333333333</v>
+      </c>
+      <c r="C9" s="0">
+        <v>0.55544016392379192</v>
+      </c>
+      <c r="D9" s="0">
+        <v>1916.5333333333333</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0">
+        <v>1941.6666666666667</v>
+      </c>
+      <c r="C10" s="0">
+        <v>0.67153169573050431</v>
+      </c>
+      <c r="D10" s="0">
+        <v>2466.1333333333332</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0">
+        <v>2547.6666666666665</v>
+      </c>
+      <c r="C11" s="0">
+        <v>0.7684038831559602</v>
+      </c>
+      <c r="D11" s="0">
+        <v>2874</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0">
+        <v>1824.5999999999999</v>
+      </c>
+      <c r="C12" s="0">
+        <v>0.67999629668559691</v>
+      </c>
+      <c r="D12" s="0">
+        <v>2184.8000000000002</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0">
+        <v>2003.6666666666667</v>
+      </c>
+      <c r="C13" s="0">
+        <v>0.37525641370641527</v>
+      </c>
+      <c r="D13" s="0">
+        <v>3343.8000000000002</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0">
+        <v>1267.0666666666666</v>
+      </c>
+      <c r="C14" s="0">
+        <v>0.46931257742580534</v>
+      </c>
+      <c r="D14" s="0">
+        <v>1699.6666666666667</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0">
+        <v>2813.0666666666666</v>
+      </c>
+      <c r="C15" s="0">
+        <v>0.5903954593483286</v>
+      </c>
+      <c r="D15" s="0">
+        <v>3301</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0">
+        <v>2297.0666666666666</v>
+      </c>
+      <c r="C16" s="0">
+        <v>0.46374469296852122</v>
+      </c>
+      <c r="D16" s="0">
+        <v>3256.9333333333334</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0">
+        <v>2313.1333333333332</v>
+      </c>
+      <c r="C17" s="0">
+        <v>0.48157127748074874</v>
+      </c>
+      <c r="D17" s="0">
+        <v>3285.1999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edicion de la nueva base
</commit_message>
<xml_diff>
--- a/Proyecto/tablaIndexada.xlsx
+++ b/Proyecto/tablaIndexada.xlsx
@@ -169,13 +169,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>25807.799999999999</v>
+        <v>8932.4666666666672</v>
       </c>
       <c r="C3" s="0">
-        <v>0.73429161795004161</v>
+        <v>0.81458949777723322</v>
       </c>
       <c r="D3" s="0">
-        <v>26172.933333333334</v>
+        <v>9051.5333333333328</v>
       </c>
     </row>
     <row r="4">
@@ -183,13 +183,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="0">
-        <v>19429.666666666668</v>
+        <v>6715.9333333333334</v>
       </c>
       <c r="C4" s="0">
-        <v>0.32455122819333565</v>
+        <v>0.34018086301823247</v>
       </c>
       <c r="D4" s="0">
-        <v>26707.466666666667</v>
+        <v>9250.4666666666672</v>
       </c>
     </row>
     <row r="5">
@@ -197,13 +197,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="0">
-        <v>20671.133333333335</v>
+        <v>7165.1999999999998</v>
       </c>
       <c r="C5" s="0">
-        <v>0.29826002382035383</v>
+        <v>0.3041257114962968</v>
       </c>
       <c r="D5" s="0">
-        <v>31799.333333333332</v>
+        <v>11035.4</v>
       </c>
     </row>
     <row r="6">
@@ -211,13 +211,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="0">
-        <v>21676.200000000001</v>
+        <v>7989.5333333333338</v>
       </c>
       <c r="C6" s="0">
-        <v>0.20807725801160448</v>
+        <v>0.17550673043891526</v>
       </c>
       <c r="D6" s="0">
-        <v>50862.73333333333</v>
+        <v>18996.333333333332</v>
       </c>
     </row>
     <row r="7">
@@ -225,13 +225,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="0">
-        <v>37003.866666666669</v>
+        <v>13822.799999999999</v>
       </c>
       <c r="C7" s="0">
-        <v>0.37160488014689447</v>
+        <v>0.42419100321698655</v>
       </c>
       <c r="D7" s="0">
-        <v>55862.066666666666</v>
+        <v>19708.933333333334</v>
       </c>
     </row>
     <row r="8">
@@ -239,13 +239,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="0">
-        <v>53698.199999999997</v>
+        <v>17924.799999999999</v>
       </c>
       <c r="C8" s="0">
-        <v>0.64439172539689704</v>
+        <v>0.64695149929858065</v>
       </c>
       <c r="D8" s="0">
-        <v>59989.800000000003</v>
+        <v>20164.599999999999</v>
       </c>
     </row>
     <row r="9">
@@ -253,13 +253,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="0">
-        <v>29502.133333333335</v>
+        <v>10624.666666666666</v>
       </c>
       <c r="C9" s="0">
-        <v>0.50950792555277657</v>
+        <v>0.51569465887054156</v>
       </c>
       <c r="D9" s="0">
-        <v>34285.666666666664</v>
+        <v>13374.533333333333</v>
       </c>
     </row>
     <row r="10">
@@ -267,13 +267,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="0">
-        <v>38051</v>
+        <v>14527.933333333332</v>
       </c>
       <c r="C10" s="0">
-        <v>0.47053120872272763</v>
+        <v>0.55620997233010594</v>
       </c>
       <c r="D10" s="0">
-        <v>58158.666666666664</v>
+        <v>21383.533333333333</v>
       </c>
     </row>
     <row r="11">
@@ -281,13 +281,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="0">
-        <v>60913.066666666666</v>
+        <v>22070.200000000001</v>
       </c>
       <c r="C11" s="0">
-        <v>0.66077547877133602</v>
+        <v>0.73979512088145361</v>
       </c>
       <c r="D11" s="0">
-        <v>70187.333333333328</v>
+        <v>24145.599999999999</v>
       </c>
     </row>
     <row r="12">
@@ -295,13 +295,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="0">
-        <v>47195.26666666667</v>
+        <v>16753.133333333335</v>
       </c>
       <c r="C12" s="0">
-        <v>0.66529337018817691</v>
+        <v>0.71573005781973198</v>
       </c>
       <c r="D12" s="0">
-        <v>55479.466666666667</v>
+        <v>19591.733333333334</v>
       </c>
     </row>
     <row r="13">
@@ -309,13 +309,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="0">
-        <v>45273.73333333333</v>
+        <v>16583.866666666665</v>
       </c>
       <c r="C13" s="0">
-        <v>0.41651029810249568</v>
+        <v>0.40567172762762926</v>
       </c>
       <c r="D13" s="0">
-        <v>70786.866666666669</v>
+        <v>27256.133333333335</v>
       </c>
     </row>
     <row r="14">
@@ -323,13 +323,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="0">
-        <v>37111.066666666666</v>
+        <v>12498.266666666666</v>
       </c>
       <c r="C14" s="0">
-        <v>0.33966077755917479</v>
+        <v>0.39298358244176668</v>
       </c>
       <c r="D14" s="0">
-        <v>60150.133333333331</v>
+        <v>18932.400000000001</v>
       </c>
     </row>
     <row r="15">
@@ -337,13 +337,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="0">
-        <v>45022.26666666667</v>
+        <v>17679.200000000001</v>
       </c>
       <c r="C15" s="0">
-        <v>0.42656050553002661</v>
+        <v>0.45222541611648842</v>
       </c>
       <c r="D15" s="0">
-        <v>54791.599999999999</v>
+        <v>21893.866666666665</v>
       </c>
     </row>
     <row r="16">
@@ -351,13 +351,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="0">
-        <v>75905.866666666669</v>
+        <v>24116.066666666666</v>
       </c>
       <c r="C16" s="0">
-        <v>0.47744600035821783</v>
+        <v>0.48426089877576123</v>
       </c>
       <c r="D16" s="0">
-        <v>96342.266666666663</v>
+        <v>31433.200000000001</v>
       </c>
     </row>
     <row r="17">
@@ -365,13 +365,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="0">
-        <v>55975.066666666666</v>
+        <v>20331.466666666667</v>
       </c>
       <c r="C17" s="0">
-        <v>0.36120323986590996</v>
+        <v>0.43050183458027658</v>
       </c>
       <c r="D17" s="0">
-        <v>87390.933333333334</v>
+        <v>30325.799999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>